<commit_message>
cambiado excel de referencia
</commit_message>
<xml_diff>
--- a/proyecto/Proyecto.xlsx
+++ b/proyecto/Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pabloarranzropero/workspace-AA/proyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBAE7B3-044A-434B-9933-4ABA09F241A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6BA85E-96E2-EC47-ABCD-3340803D50D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480" xr2:uid="{C973FD6A-279B-E940-A142-77E1A770ECF6}"/>
   </bookViews>
@@ -884,7 +884,7 @@
   <dimension ref="A1:P1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,13 +1058,12 @@
       <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>

</xml_diff>